<commit_message>
added comments and solutions
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhruv\google drive\IISER\Turing Club\Hackathon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhruv\Programs\HTML Javascript\Darwin Hackathon\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA6295B-545E-4725-8A66-5BC1F3DB6C69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC7DA77-98E3-422A-95A7-ED0316F36912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -614,9 +613,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="77" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1433,7 +1432,7 @@
         <v>10</v>
       </c>
       <c r="J21" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K21" s="4">
         <v>5</v>
@@ -1518,7 +1517,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="9">
         <f>SUM(E21:K21)</f>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -1548,7 +1547,7 @@
       <c r="V23" s="9"/>
       <c r="W23" s="10">
         <f t="shared" ref="W23" si="3">SUM(A23:V23)</f>
-        <v>285</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="29" x14ac:dyDescent="0.35">

</xml_diff>